<commit_message>
Component counts for 3 sets.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marten\Code\VCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD98C2A-F5A4-46D9-A48E-36B385B46568}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F46ED9D-1339-4511-BDD7-46ADA1A9F98A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25545" windowHeight="18120" xr2:uid="{D120D5B5-606E-49B3-8DBD-703CF8BB7901}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="129">
   <si>
     <t>Comment</t>
   </si>
@@ -409,6 +409,9 @@
   </si>
   <si>
     <t>D1, D2,D5</t>
+  </si>
+  <si>
+    <t>3X</t>
   </si>
 </sst>
 </file>
@@ -931,10 +934,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C91B5EE9-B2ED-4BDE-8F18-7EEE0F5A4ED1}">
-  <dimension ref="B3:I39"/>
+  <dimension ref="B3:K39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,7 +950,7 @@
     <col min="7" max="7" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -972,8 +975,11 @@
       <c r="I3" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="4" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K3" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
         <v>50</v>
       </c>
@@ -999,8 +1005,12 @@
         <f>G4*H4</f>
         <v>1.452</v>
       </c>
-    </row>
-    <row r="5" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K4" s="3">
+        <f>3*G4</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>52</v>
       </c>
@@ -1026,8 +1036,12 @@
         <f t="shared" ref="I5:I38" si="0">G5*H5</f>
         <v>0.52800000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K5" s="3">
+        <f t="shared" ref="K5:K38" si="1">3*G5</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1053,8 +1067,12 @@
         <f t="shared" si="0"/>
         <v>0.16800000000000001</v>
       </c>
-    </row>
-    <row r="7" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K6" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>55</v>
       </c>
@@ -1080,8 +1098,12 @@
         <f t="shared" si="0"/>
         <v>0.10200000000000001</v>
       </c>
-    </row>
-    <row r="8" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K7" s="3">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -1107,8 +1129,12 @@
         <f t="shared" si="0"/>
         <v>5.6000000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K8" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>22</v>
       </c>
@@ -1132,8 +1158,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K9" s="3">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
         <v>61</v>
       </c>
@@ -1157,8 +1187,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K10" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>65</v>
       </c>
@@ -1184,8 +1218,12 @@
         <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K11" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>70</v>
       </c>
@@ -1211,8 +1249,12 @@
         <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K12" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
         <v>74</v>
       </c>
@@ -1238,8 +1280,12 @@
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K13" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
         <v>32</v>
       </c>
@@ -1265,8 +1311,12 @@
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K14" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1292,8 +1342,12 @@
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K15" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
@@ -1319,8 +1373,12 @@
         <f t="shared" si="0"/>
         <v>0.23399999999999999</v>
       </c>
-    </row>
-    <row r="17" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K16" s="3">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>27</v>
       </c>
@@ -1346,8 +1404,12 @@
         <f t="shared" si="0"/>
         <v>0.156</v>
       </c>
-    </row>
-    <row r="18" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K17" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>80</v>
       </c>
@@ -1373,8 +1435,12 @@
         <f t="shared" si="0"/>
         <v>0.156</v>
       </c>
-    </row>
-    <row r="19" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K18" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>82</v>
       </c>
@@ -1400,8 +1466,12 @@
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-    </row>
-    <row r="20" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K19" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>84</v>
       </c>
@@ -1427,8 +1497,12 @@
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-    </row>
-    <row r="21" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K20" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>86</v>
       </c>
@@ -1454,8 +1528,12 @@
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-    </row>
-    <row r="22" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K21" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>34</v>
       </c>
@@ -1481,8 +1559,12 @@
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-    </row>
-    <row r="23" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K22" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>31</v>
       </c>
@@ -1508,8 +1590,12 @@
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-    </row>
-    <row r="24" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K23" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>90</v>
       </c>
@@ -1535,8 +1621,12 @@
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-    </row>
-    <row r="25" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K24" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>6</v>
       </c>
@@ -1562,8 +1652,12 @@
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-    </row>
-    <row r="26" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K25" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>93</v>
       </c>
@@ -1589,8 +1683,12 @@
         <f t="shared" si="0"/>
         <v>1.2</v>
       </c>
-    </row>
-    <row r="27" spans="2:9" ht="42" x14ac:dyDescent="0.25">
+      <c r="K26" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="42" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>36</v>
       </c>
@@ -1616,8 +1714,12 @@
         <f t="shared" si="0"/>
         <v>0.878</v>
       </c>
-    </row>
-    <row r="28" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K27" s="3">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>95</v>
       </c>
@@ -1643,8 +1745,12 @@
         <f t="shared" si="0"/>
         <v>2.7</v>
       </c>
-    </row>
-    <row r="29" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K28" s="3">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>100</v>
       </c>
@@ -1670,8 +1776,12 @@
         <f t="shared" si="0"/>
         <v>0.496</v>
       </c>
-    </row>
-    <row r="30" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K29" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>105</v>
       </c>
@@ -1697,8 +1807,12 @@
         <f t="shared" si="0"/>
         <v>0.85399999999999998</v>
       </c>
-    </row>
-    <row r="31" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K30" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>45</v>
       </c>
@@ -1725,8 +1839,12 @@
         <f t="shared" si="0"/>
         <v>3.0393600000000003</v>
       </c>
-    </row>
-    <row r="32" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K31" s="3">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
         <v>21</v>
       </c>
@@ -1752,8 +1870,12 @@
         <f t="shared" si="0"/>
         <v>0.15</v>
       </c>
-    </row>
-    <row r="33" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K32" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
         <v>115</v>
       </c>
@@ -1780,8 +1902,12 @@
         <f t="shared" si="0"/>
         <v>0.51604000000000005</v>
       </c>
-    </row>
-    <row r="34" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K33" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
         <v>6</v>
       </c>
@@ -1808,8 +1934,12 @@
         <f t="shared" si="0"/>
         <v>3.6883280000000003</v>
       </c>
-    </row>
-    <row r="35" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K34" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
         <v>125</v>
       </c>
@@ -1833,8 +1963,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:9" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="K35" s="3">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
         <v>61</v>
       </c>
@@ -1858,8 +1992,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K36" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
         <v>32</v>
       </c>
@@ -1885,8 +2023,12 @@
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-    </row>
-    <row r="38" spans="2:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="K37" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" ht="21" x14ac:dyDescent="0.25">
       <c r="B38" s="8" t="s">
         <v>31</v>
       </c>
@@ -1912,8 +2054,12 @@
         <f t="shared" si="0"/>
         <v>7.8E-2</v>
       </c>
-    </row>
-    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="K38" s="3">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
         <v>40</v>
       </c>

</xml_diff>